<commit_message>
Import DB and add some DTOs
</commit_message>
<xml_diff>
--- a/BTL.xlsx
+++ b/BTL.xlsx
@@ -8,217 +8,41 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CNTT_Shared\OOP\OOP_Summer_2025_Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD9938DD-A010-47C2-A292-20D2C502657B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5449E898-1BA2-46F5-AE62-1B916D83B30A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Overall Architecture" sheetId="1" r:id="rId1"/>
-    <sheet name="Java App" sheetId="3" r:id="rId2"/>
-    <sheet name="Timeline" sheetId="2" r:id="rId3"/>
+    <sheet name="UML Diagram" sheetId="5" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>HTTP / HTTPS GET+ POST</t>
   </si>
   <si>
-    <t>com.example.library</t>
-  </si>
-  <si>
-    <t>├── model         # OOP domain classes (Book, User, etc.)</t>
-  </si>
-  <si>
-    <t>├── service       # Business logic (borrowing, returning)</t>
-  </si>
-  <si>
-    <t>├── controller    # REST or Web controllers (Spring endpoints)</t>
-  </si>
-  <si>
-    <t>├── config        # DB config, exception handling, CORS, etc.</t>
-  </si>
-  <si>
-    <t>└── LibraryApp    # Main Spring Boot application class</t>
-  </si>
-  <si>
-    <t>├── repository    # Data access (SQLite + JDBC)</t>
-  </si>
-  <si>
-    <t>// Book.java</t>
-  </si>
-  <si>
-    <t>public class Book {</t>
-  </si>
-  <si>
-    <t xml:space="preserve">    private int id;</t>
-  </si>
-  <si>
-    <t xml:space="preserve">    private String title;</t>
-  </si>
-  <si>
-    <t xml:space="preserve">    private String author;</t>
-  </si>
-  <si>
-    <t xml:space="preserve">    private boolean isBorrowed;</t>
-  </si>
-  <si>
-    <t xml:space="preserve">    // Getters, setters, constructors</t>
-  </si>
-  <si>
     <t>}</t>
-  </si>
-  <si>
-    <t>public class BookRepository {</t>
-  </si>
-  <si>
-    <t xml:space="preserve">    private final Connection conn;</t>
-  </si>
-  <si>
-    <t xml:space="preserve">    public BookRepository(Connection conn) { this.conn = conn; }</t>
-  </si>
-  <si>
-    <t xml:space="preserve">    public List&lt;Book&gt; findAll() throws SQLException { ... }</t>
-  </si>
-  <si>
-    <t xml:space="preserve">    public void save(Book book) { ... }</t>
-  </si>
-  <si>
-    <t xml:space="preserve">    public void delete(int id) { ... }</t>
-  </si>
-  <si>
-    <t>@Service</t>
-  </si>
-  <si>
-    <t>public class LibraryService {</t>
-  </si>
-  <si>
-    <t xml:space="preserve">    @Autowired private BookRepository bookRepo;</t>
-  </si>
-  <si>
-    <t xml:space="preserve">    public List&lt;Book&gt; listBooks() { return bookRepo.findAll(); }</t>
-  </si>
-  <si>
-    <t xml:space="preserve">    public void borrowBook(int id) {</t>
-  </si>
-  <si>
-    <t xml:space="preserve">        Book book = bookRepo.findById(id);</t>
-  </si>
-  <si>
-    <t xml:space="preserve">        if (book.isBorrowed()) throw new IllegalStateException("Already borrowed");</t>
-  </si>
-  <si>
-    <t xml:space="preserve">        book.setBorrowed(true);</t>
-  </si>
-  <si>
-    <t xml:space="preserve">        bookRepo.update(book);</t>
-  </si>
-  <si>
-    <t xml:space="preserve">    }</t>
-  </si>
-  <si>
-    <t>@Repository</t>
-  </si>
-  <si>
-    <t>@RestController</t>
-  </si>
-  <si>
-    <t>@RequestMapping("/api/books")</t>
-  </si>
-  <si>
-    <t>public class BookController {</t>
-  </si>
-  <si>
-    <t xml:space="preserve">    @Autowired private LibraryService service;</t>
-  </si>
-  <si>
-    <t xml:space="preserve">    @GetMapping public List&lt;Book&gt; getAll() { return service.listBooks(); }</t>
-  </si>
-  <si>
-    <t xml:space="preserve">    @PostMapping("/{id}/borrow")</t>
-  </si>
-  <si>
-    <t xml:space="preserve">    public void borrow(@PathVariable int id) {</t>
-  </si>
-  <si>
-    <t xml:space="preserve">        service.borrowBook(id);</t>
-  </si>
-  <si>
-    <t>@Configuration</t>
-  </si>
-  <si>
-    <t>public class SQLiteConfig {</t>
-  </si>
-  <si>
-    <t xml:space="preserve">    @Bean</t>
-  </si>
-  <si>
-    <t xml:space="preserve">    public Connection sqliteConnection() throws SQLException {</t>
-  </si>
-  <si>
-    <t xml:space="preserve">        return DriverManager.getConnection("jdbc:sqlite:/opt/data/library.db");</t>
-  </si>
-  <si>
-    <t>@SpringBootApplication</t>
-  </si>
-  <si>
-    <t>public class LibraryApp {</t>
-  </si>
-  <si>
-    <t xml:space="preserve">    public static void main(String[] args) {</t>
-  </si>
-  <si>
-    <t xml:space="preserve">        SpringApplication.run(LibraryApp.class, args);</t>
-  </si>
-  <si>
-    <t>library-app/</t>
-  </si>
-  <si>
-    <t>├── src/</t>
-  </si>
-  <si>
-    <t>│   ├── Book.java             # OOP model class</t>
-  </si>
-  <si>
-    <t>│   ├── BookDAO.java          # Reads/writes to SQLite</t>
-  </si>
-  <si>
-    <t>│   ├── LibraryServer.java    # Starts the web server</t>
-  </si>
-  <si>
-    <t>│   ├── HtmlHandler.java      # Handles incoming HTTP requests</t>
-  </si>
-  <si>
-    <t>├── web/</t>
-  </si>
-  <si>
-    <t>│   ├── index.html            # Main menu</t>
-  </si>
-  <si>
-    <t>│   ├── list.html             # View books</t>
-  </si>
-  <si>
-    <t>│   └── add.html              # Add book form</t>
-  </si>
-  <si>
-    <t>├── lib/</t>
-  </si>
-  <si>
-    <t>│   ├── sqlite-jdbc.jar       # JDBC SQLite driver</t>
-  </si>
-  <si>
-    <t>│   └── nanohttpd.jar         # Lightweight embedded HTTP server</t>
-  </si>
-  <si>
-    <t>├── library.db                # SQLite DB file</t>
   </si>
   <si>
     <t>public enum ActionType {</t>
@@ -1373,6 +1197,2863 @@
         </a:fillRef>
         <a:effectRef idx="0">
           <a:schemeClr val="accent6"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>361950</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>95249</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>523875</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>47624</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="Rectangle 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{497A7EE8-4B33-B00F-BF1F-B680A3F3DE1B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="361950" y="285749"/>
+          <a:ext cx="2600325" cy="3762375"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:sysClr val="windowText" lastClr="000000"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent6"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent6"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100"/>
+            <a:t>package model</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100"/>
+            <a:t>abstract class User</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100"/>
+            <a:t>- String userId</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100"/>
+            <a:t>- String email</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100"/>
+            <a:t>- String password</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100"/>
+            <a:t>- List&lt;String&gt; borrowedBookIds</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100"/>
+            <a:t>+ User(String userId, String email, String password)</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100"/>
+            <a:t>+ String getUserId()</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100"/>
+            <a:t>+ void setUserId(String userId)</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100"/>
+            <a:t>+ String getEmail()</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100"/>
+            <a:t>+ void setEmail(String email)</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100"/>
+            <a:t>+ String getPassword()</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100"/>
+            <a:t>+ void setPassword(String password)</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100"/>
+            <a:t>+ List&lt;String&gt; getBorrowedBookIds()</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100"/>
+            <a:t>+ void setBorrowedBookIds(List&lt;String&gt; borrowedBookIds)</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100"/>
+            <a:t>+ void borrowBook(String bookId)</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100"/>
+            <a:t>+ void returnBook(String bookId)</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100"/>
+            <a:t>+ abstract String getRole()</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100"/>
+            <a:t>// @Override String toString()</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-GB" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>495301</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>158751</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>174625</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="4" name="Rectangle 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A9375DC4-3C84-4A87-B1EB-A725C1CF93F8}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4114801" y="2028825"/>
+          <a:ext cx="3886200" cy="1384300"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:sysClr val="windowText" lastClr="000000"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent6"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent6"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100"/>
+            <a:t>package model</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100"/>
+            <a:t>class Member extends User</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100"/>
+            <a:t>+ Member(String userId, String email, String password)</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100"/>
+            <a:t>+ void borrowBook(String bookId) // redefined with extra check</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100"/>
+            <a:t>+ void returnBook(String bookId) // redefined</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100"/>
+            <a:t>+ String getRole() // @Override</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100"/>
+            <a:t>+ String toString() // @Override</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-GB" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>27781</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>134936</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>555624</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>23811</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="3073" name="Text Box 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{94DFCBEA-719D-0D2A-6D95-344C1FE63182}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1">
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="4278312" y="325436"/>
+          <a:ext cx="3563937" cy="1412875"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:miter lim="800000"/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="18288" rIns="0" bIns="0" anchor="t" upright="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l" rtl="0">
+            <a:defRPr sz="1000"/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Calibri"/>
+              <a:ea typeface="Calibri"/>
+              <a:cs typeface="Calibri"/>
+            </a:rPr>
+            <a:t>package model</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l" rtl="0">
+            <a:defRPr sz="1000"/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Calibri"/>
+              <a:ea typeface="Calibri"/>
+              <a:cs typeface="Calibri"/>
+            </a:rPr>
+            <a:t>class Admin extends User</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l" rtl="0">
+            <a:defRPr sz="1000"/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Calibri"/>
+              <a:ea typeface="Calibri"/>
+              <a:cs typeface="Calibri"/>
+            </a:rPr>
+            <a:t>+ Admin(String userId, String email, String password)</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l" rtl="0">
+            <a:defRPr sz="1000"/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Calibri"/>
+              <a:ea typeface="Calibri"/>
+              <a:cs typeface="Calibri"/>
+            </a:rPr>
+            <a:t>+ String getRole() // @Override</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l" rtl="0">
+            <a:defRPr sz="1000"/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Calibri"/>
+              <a:ea typeface="Calibri"/>
+              <a:cs typeface="Calibri"/>
+            </a:rPr>
+            <a:t>+ void addBook(Book book, LibraryManager manager)</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l" rtl="0">
+            <a:defRPr sz="1000"/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Calibri"/>
+              <a:ea typeface="Calibri"/>
+              <a:cs typeface="Calibri"/>
+            </a:rPr>
+            <a:t>+ void removeBook(Book book, LibraryManager manager)</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l" rtl="0">
+            <a:defRPr sz="1000"/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Calibri"/>
+              <a:ea typeface="Calibri"/>
+              <a:cs typeface="Calibri"/>
+            </a:rPr>
+            <a:t>+ void viewBorrowedBooks(Member member)</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l" rtl="0">
+            <a:defRPr sz="1000"/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="Calibri"/>
+              <a:cs typeface="Calibri"/>
+            </a:rPr>
+            <a:t>+ void removeUser(String userId, LibraryManager manager)   </a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>164224</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>30109</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>195974</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>125359</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="3074" name="Text Box 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{090049A6-2ABC-D1A3-A0DF-10FB5886DAAC}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1">
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="9886293" y="30109"/>
+          <a:ext cx="3677526" cy="3839560"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:miter lim="800000"/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="18288" rIns="0" bIns="0" anchor="t" upright="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l" rtl="0">
+            <a:defRPr sz="1000"/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Calibri"/>
+              <a:ea typeface="Calibri"/>
+              <a:cs typeface="Calibri"/>
+            </a:rPr>
+            <a:t>package model</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l" rtl="0">
+            <a:defRPr sz="1000"/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Calibri"/>
+              <a:ea typeface="Calibri"/>
+              <a:cs typeface="Calibri"/>
+            </a:rPr>
+            <a:t>class Record</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l" rtl="0">
+            <a:defRPr sz="1000"/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Calibri"/>
+              <a:ea typeface="Calibri"/>
+              <a:cs typeface="Calibri"/>
+            </a:rPr>
+            <a:t>- String recordId</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l" rtl="0">
+            <a:defRPr sz="1000"/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Calibri"/>
+              <a:ea typeface="Calibri"/>
+              <a:cs typeface="Calibri"/>
+            </a:rPr>
+            <a:t>- LocalDateTime timestamp</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l" rtl="0">
+            <a:defRPr sz="1000"/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Calibri"/>
+              <a:ea typeface="Calibri"/>
+              <a:cs typeface="Calibri"/>
+            </a:rPr>
+            <a:t>- String userId</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l" rtl="0">
+            <a:defRPr sz="1000"/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Calibri"/>
+              <a:ea typeface="Calibri"/>
+              <a:cs typeface="Calibri"/>
+            </a:rPr>
+            <a:t>- String bookId</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l" rtl="0">
+            <a:defRPr sz="1000"/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Calibri"/>
+              <a:ea typeface="Calibri"/>
+              <a:cs typeface="Calibri"/>
+            </a:rPr>
+            <a:t>- ActionType action</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l" rtl="0">
+            <a:defRPr sz="1000"/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Calibri"/>
+              <a:ea typeface="Calibri"/>
+              <a:cs typeface="Calibri"/>
+            </a:rPr>
+            <a:t>+ Record(String recordId, String userId, String bookId, ActionType action)</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l" rtl="0">
+            <a:defRPr sz="1000"/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Calibri"/>
+              <a:ea typeface="Calibri"/>
+              <a:cs typeface="Calibri"/>
+            </a:rPr>
+            <a:t>+ String getRecordId()</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l" rtl="0">
+            <a:defRPr sz="1000"/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Calibri"/>
+              <a:ea typeface="Calibri"/>
+              <a:cs typeface="Calibri"/>
+            </a:rPr>
+            <a:t>+ void setRecordId(String recordId)</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l" rtl="0">
+            <a:defRPr sz="1000"/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Calibri"/>
+              <a:ea typeface="Calibri"/>
+              <a:cs typeface="Calibri"/>
+            </a:rPr>
+            <a:t>+ LocalDateTime getTimestamp()</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l" rtl="0">
+            <a:defRPr sz="1000"/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Calibri"/>
+              <a:ea typeface="Calibri"/>
+              <a:cs typeface="Calibri"/>
+            </a:rPr>
+            <a:t>+ void setTimestamp(LocalDateTime timestamp)</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l" rtl="0">
+            <a:defRPr sz="1000"/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Calibri"/>
+              <a:ea typeface="Calibri"/>
+              <a:cs typeface="Calibri"/>
+            </a:rPr>
+            <a:t>+ String getUserId()</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l" rtl="0">
+            <a:defRPr sz="1000"/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Calibri"/>
+              <a:ea typeface="Calibri"/>
+              <a:cs typeface="Calibri"/>
+            </a:rPr>
+            <a:t>+ void setUserId(String userId)</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l" rtl="0">
+            <a:defRPr sz="1000"/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Calibri"/>
+              <a:ea typeface="Calibri"/>
+              <a:cs typeface="Calibri"/>
+            </a:rPr>
+            <a:t>+ String getBookId()</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l" rtl="0">
+            <a:defRPr sz="1000"/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Calibri"/>
+              <a:ea typeface="Calibri"/>
+              <a:cs typeface="Calibri"/>
+            </a:rPr>
+            <a:t>+ void setBookId(String bookId)</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l" rtl="0">
+            <a:defRPr sz="1000"/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Calibri"/>
+              <a:ea typeface="Calibri"/>
+              <a:cs typeface="Calibri"/>
+            </a:rPr>
+            <a:t>+ ActionType getAction()</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l" rtl="0">
+            <a:defRPr sz="1000"/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Calibri"/>
+              <a:ea typeface="Calibri"/>
+              <a:cs typeface="Calibri"/>
+            </a:rPr>
+            <a:t>+ void setAction(ActionType action)</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l" rtl="0">
+            <a:defRPr sz="1000"/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Calibri"/>
+              <a:ea typeface="Calibri"/>
+              <a:cs typeface="Calibri"/>
+            </a:rPr>
+            <a:t>+ boolean isReturned()</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l" rtl="0">
+            <a:defRPr sz="1000"/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Calibri"/>
+              <a:ea typeface="Calibri"/>
+              <a:cs typeface="Calibri"/>
+            </a:rPr>
+            <a:t>+ String toString() // @Override</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l" rtl="0">
+            <a:defRPr sz="1000"/>
+          </a:pPr>
+          <a:endParaRPr lang="en-GB" sz="1100" b="0" i="0" u="none" strike="noStrike" baseline="0">
+            <a:solidFill>
+              <a:srgbClr val="000000"/>
+            </a:solidFill>
+            <a:latin typeface="Calibri"/>
+            <a:ea typeface="Calibri"/>
+            <a:cs typeface="Calibri"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>319086</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>5556</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>303212</xdr:colOff>
+      <xdr:row>53</xdr:row>
+      <xdr:rowOff>108799</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="3075" name="Text Box 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A7078BE6-C975-386A-5D29-48B167730F9E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1">
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="3962399" y="5339556"/>
+          <a:ext cx="6056313" cy="4865743"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:miter lim="800000"/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="18288" rIns="0" bIns="0" anchor="t" upright="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l" rtl="0">
+            <a:defRPr sz="1000"/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Calibri"/>
+              <a:ea typeface="Calibri"/>
+              <a:cs typeface="Calibri"/>
+            </a:rPr>
+            <a:t>package model</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l" rtl="0">
+            <a:defRPr sz="1000"/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Calibri"/>
+              <a:ea typeface="Calibri"/>
+              <a:cs typeface="Calibri"/>
+            </a:rPr>
+            <a:t>class Book</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l" rtl="0">
+            <a:defRPr sz="1000"/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Calibri"/>
+              <a:ea typeface="Calibri"/>
+              <a:cs typeface="Calibri"/>
+            </a:rPr>
+            <a:t>- String bookId</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l" rtl="0">
+            <a:defRPr sz="1000"/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Calibri"/>
+              <a:ea typeface="Calibri"/>
+              <a:cs typeface="Calibri"/>
+            </a:rPr>
+            <a:t>- String title</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l" rtl="0">
+            <a:defRPr sz="1000"/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Calibri"/>
+              <a:ea typeface="Calibri"/>
+              <a:cs typeface="Calibri"/>
+            </a:rPr>
+            <a:t>- String author</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l" rtl="0">
+            <a:defRPr sz="1000"/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Calibri"/>
+              <a:ea typeface="Calibri"/>
+              <a:cs typeface="Calibri"/>
+            </a:rPr>
+            <a:t>- String publisher</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l" rtl="0">
+            <a:defRPr sz="1000"/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Calibri"/>
+              <a:ea typeface="Calibri"/>
+              <a:cs typeface="Calibri"/>
+            </a:rPr>
+            <a:t>- int yearPublished</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l" rtl="0">
+            <a:defRPr sz="1000"/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Calibri"/>
+              <a:ea typeface="Calibri"/>
+              <a:cs typeface="Calibri"/>
+            </a:rPr>
+            <a:t>- List&lt;String&gt; genres</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l" rtl="0">
+            <a:defRPr sz="1000"/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Calibri"/>
+              <a:ea typeface="Calibri"/>
+              <a:cs typeface="Calibri"/>
+            </a:rPr>
+            <a:t>- int borrowCount</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l" rtl="0">
+            <a:defRPr sz="1000"/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Calibri"/>
+              <a:ea typeface="Calibri"/>
+              <a:cs typeface="Calibri"/>
+            </a:rPr>
+            <a:t>- String imgUrl</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l" rtl="0">
+            <a:defRPr sz="1000"/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Calibri"/>
+              <a:ea typeface="Calibri"/>
+              <a:cs typeface="Calibri"/>
+            </a:rPr>
+            <a:t>+ Book(String bookId, String title, String author, String publisher, int yearPublished, List&lt;String&gt; genres, String imgUrl)</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l" rtl="0">
+            <a:defRPr sz="1000"/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Calibri"/>
+              <a:ea typeface="Calibri"/>
+              <a:cs typeface="Calibri"/>
+            </a:rPr>
+            <a:t>+ String getBookId()</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l" rtl="0">
+            <a:defRPr sz="1000"/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Calibri"/>
+              <a:ea typeface="Calibri"/>
+              <a:cs typeface="Calibri"/>
+            </a:rPr>
+            <a:t>+ void setBookId(String bookId)</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l" rtl="0">
+            <a:defRPr sz="1000"/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Calibri"/>
+              <a:ea typeface="Calibri"/>
+              <a:cs typeface="Calibri"/>
+            </a:rPr>
+            <a:t>+ String getTitle()</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l" rtl="0">
+            <a:defRPr sz="1000"/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Calibri"/>
+              <a:ea typeface="Calibri"/>
+              <a:cs typeface="Calibri"/>
+            </a:rPr>
+            <a:t>+ void setTitle(String title)</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l" rtl="0">
+            <a:defRPr sz="1000"/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Calibri"/>
+              <a:ea typeface="Calibri"/>
+              <a:cs typeface="Calibri"/>
+            </a:rPr>
+            <a:t>+ String getAuthor()</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l" rtl="0">
+            <a:defRPr sz="1000"/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Calibri"/>
+              <a:ea typeface="Calibri"/>
+              <a:cs typeface="Calibri"/>
+            </a:rPr>
+            <a:t>+ void setAuthor(String author)</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l" rtl="0">
+            <a:defRPr sz="1000"/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Calibri"/>
+              <a:ea typeface="Calibri"/>
+              <a:cs typeface="Calibri"/>
+            </a:rPr>
+            <a:t>+ String getPublisher()</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l" rtl="0">
+            <a:defRPr sz="1000"/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Calibri"/>
+              <a:ea typeface="Calibri"/>
+              <a:cs typeface="Calibri"/>
+            </a:rPr>
+            <a:t>+ void setPublisher(String publisher)</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l" rtl="0">
+            <a:defRPr sz="1000"/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Calibri"/>
+              <a:ea typeface="Calibri"/>
+              <a:cs typeface="Calibri"/>
+            </a:rPr>
+            <a:t>+ int getYearPublished()</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l" rtl="0">
+            <a:defRPr sz="1000"/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Calibri"/>
+              <a:ea typeface="Calibri"/>
+              <a:cs typeface="Calibri"/>
+            </a:rPr>
+            <a:t>+ void setYearPublished(int yearPublished)</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l" rtl="0">
+            <a:defRPr sz="1000"/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Calibri"/>
+              <a:ea typeface="Calibri"/>
+              <a:cs typeface="Calibri"/>
+            </a:rPr>
+            <a:t>+ List&lt;String&gt; getGenres()</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l" rtl="0">
+            <a:defRPr sz="1000"/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Calibri"/>
+              <a:ea typeface="Calibri"/>
+              <a:cs typeface="Calibri"/>
+            </a:rPr>
+            <a:t>+ void setGenres(List&lt;String&gt; genres)</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l" rtl="0">
+            <a:defRPr sz="1000"/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Calibri"/>
+              <a:ea typeface="Calibri"/>
+              <a:cs typeface="Calibri"/>
+            </a:rPr>
+            <a:t>+ int getBorrowCount()</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l" rtl="0">
+            <a:defRPr sz="1000"/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Calibri"/>
+              <a:ea typeface="Calibri"/>
+              <a:cs typeface="Calibri"/>
+            </a:rPr>
+            <a:t>+ void incrementBorrowCount()</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l" rtl="0">
+            <a:defRPr sz="1000"/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Calibri"/>
+              <a:ea typeface="Calibri"/>
+              <a:cs typeface="Calibri"/>
+            </a:rPr>
+            <a:t>+ String getImgUrl()</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l" rtl="0">
+            <a:defRPr sz="1000"/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Calibri"/>
+              <a:ea typeface="Calibri"/>
+              <a:cs typeface="Calibri"/>
+            </a:rPr>
+            <a:t>+ void setImgUrl(String imgUrl)</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l" rtl="0">
+            <a:defRPr sz="1000"/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Calibri"/>
+              <a:ea typeface="Calibri"/>
+              <a:cs typeface="Calibri"/>
+            </a:rPr>
+            <a:t>+ String toString() // @Override</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l" rtl="0">
+            <a:defRPr sz="1000"/>
+          </a:pPr>
+          <a:endParaRPr lang="en-GB" sz="1100" b="0" i="0" u="none" strike="noStrike" baseline="0">
+            <a:solidFill>
+              <a:srgbClr val="000000"/>
+            </a:solidFill>
+            <a:latin typeface="Calibri"/>
+            <a:ea typeface="Calibri"/>
+            <a:cs typeface="Calibri"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>523875</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>79373</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>27781</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>71436</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="7" name="Connector: Elbow 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5F8D69E8-84DA-DF6A-2B2C-537E4A89025E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="3073" idx="1"/>
+          <a:endCxn id="2" idx="3"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="10800000" flipV="1">
+          <a:off x="2952750" y="1031873"/>
+          <a:ext cx="1325562" cy="1135063"/>
+        </a:xfrm>
+        <a:prstGeom prst="bentConnector3">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>523875</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>71437</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>495301</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>53975</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="9" name="Connector: Elbow 8">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{70A0BB38-528E-42A6-9AED-4F5CE397E6E4}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="4" idx="1"/>
+          <a:endCxn id="2" idx="3"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="10800000">
+          <a:off x="2936875" y="2166937"/>
+          <a:ext cx="1177926" cy="554038"/>
+        </a:xfrm>
+        <a:prstGeom prst="bentConnector3">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>365125</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>79376</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>527050</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>174626</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="13" name="Rectangle 12">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EC6CF43C-AFC2-4820-93F4-862ACCD6993F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="365125" y="4270376"/>
+          <a:ext cx="2574925" cy="1238250"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:sysClr val="windowText" lastClr="000000"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent6"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent6"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100"/>
+            <a:t>package type</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100"/>
+            <a:t>enum ActionType</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100"/>
+            <a:t>+ BORROW</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100"/>
+            <a:t>+ RETURN</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100"/>
+            <a:t>+ boolean isBorrowing()</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100"/>
+            <a:t>+ boolean isReturning()</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-GB" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>161090</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>148122</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>557675</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>40391</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="3076" name="Text Box 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{817D7D72-AC3A-42C8-E4EF-1C197997F176}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1">
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="10483809" y="3958122"/>
+          <a:ext cx="4039897" cy="1606769"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:miter lim="800000"/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" wrap="square" lIns="18288" tIns="18288" rIns="0" bIns="0" anchor="t" upright="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l" rtl="0">
+            <a:defRPr sz="1000"/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Calibri"/>
+              <a:ea typeface="Calibri"/>
+              <a:cs typeface="Calibri"/>
+            </a:rPr>
+            <a:t>package dao</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l" rtl="0">
+            <a:defRPr sz="1000"/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Calibri"/>
+              <a:ea typeface="Calibri"/>
+              <a:cs typeface="Calibri"/>
+            </a:rPr>
+            <a:t>class BookDAO</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l" rtl="0">
+            <a:defRPr sz="1000"/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Calibri"/>
+              <a:ea typeface="Calibri"/>
+              <a:cs typeface="Calibri"/>
+            </a:rPr>
+            <a:t>+ void addBook(Book book)</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l" rtl="0">
+            <a:defRPr sz="1000"/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Calibri"/>
+              <a:ea typeface="Calibri"/>
+              <a:cs typeface="Calibri"/>
+            </a:rPr>
+            <a:t>+ void removeBookFromDB(String bookId)</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l" rtl="0">
+            <a:defRPr sz="1000"/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Calibri"/>
+              <a:ea typeface="Calibri"/>
+              <a:cs typeface="Calibri"/>
+            </a:rPr>
+            <a:t>+ List&lt;Book&gt; getAllBooks()</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l" rtl="0">
+            <a:defRPr sz="1000"/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Calibri"/>
+              <a:ea typeface="Calibri"/>
+              <a:cs typeface="Calibri"/>
+            </a:rPr>
+            <a:t>+ void updateBorrowCount(String bookId, int borrowCount)</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l" rtl="0">
+            <a:defRPr sz="1000"/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Calibri"/>
+              <a:ea typeface="Calibri"/>
+              <a:cs typeface="Calibri"/>
+            </a:rPr>
+            <a:t>+ Book getBookById(String bookId)</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l" rtl="0">
+            <a:defRPr sz="1000"/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Calibri"/>
+              <a:ea typeface="Calibri"/>
+              <a:cs typeface="Calibri"/>
+            </a:rPr>
+            <a:t>+ void updateBook(Book book)</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l" rtl="0">
+            <a:defRPr sz="1000"/>
+          </a:pPr>
+          <a:endParaRPr lang="en-GB" sz="1100" b="0" i="0" u="none" strike="noStrike" baseline="0">
+            <a:solidFill>
+              <a:srgbClr val="000000"/>
+            </a:solidFill>
+            <a:latin typeface="Calibri"/>
+            <a:ea typeface="Calibri"/>
+            <a:cs typeface="Calibri"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>151990</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>123580</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>94840</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>9280</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="3077" name="Text Box 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C16C284A-0104-A4EA-7621-943AE6D19A5C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1">
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="10474709" y="5648080"/>
+          <a:ext cx="2371725" cy="1028700"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:miter lim="800000"/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" wrap="square" lIns="18288" tIns="18288" rIns="0" bIns="0" anchor="t" upright="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l" rtl="0">
+            <a:defRPr sz="1000"/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Calibri"/>
+              <a:ea typeface="Calibri"/>
+              <a:cs typeface="Calibri"/>
+            </a:rPr>
+            <a:t>package dao</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l" rtl="0">
+            <a:defRPr sz="1000"/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Calibri"/>
+              <a:ea typeface="Calibri"/>
+              <a:cs typeface="Calibri"/>
+            </a:rPr>
+            <a:t>class RecordDAO</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l" rtl="0">
+            <a:defRPr sz="1000"/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Calibri"/>
+              <a:ea typeface="Calibri"/>
+              <a:cs typeface="Calibri"/>
+            </a:rPr>
+            <a:t>+ void addRecord(Record record)</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l" rtl="0">
+            <a:defRPr sz="1000"/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Calibri"/>
+              <a:ea typeface="Calibri"/>
+              <a:cs typeface="Calibri"/>
+            </a:rPr>
+            <a:t>+ List&lt;Record&gt; getAllRecords()</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l" rtl="0">
+            <a:defRPr sz="1000"/>
+          </a:pPr>
+          <a:endParaRPr lang="en-GB" sz="1100" b="0" i="0" u="none" strike="noStrike" baseline="0">
+            <a:solidFill>
+              <a:srgbClr val="000000"/>
+            </a:solidFill>
+            <a:latin typeface="Calibri"/>
+            <a:ea typeface="Calibri"/>
+            <a:cs typeface="Calibri"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>221114</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>107560</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>559594</xdr:colOff>
+      <xdr:row>45</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="3078" name="Text Box 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0ACF80C0-4237-219F-EBCF-63C5C3B5169E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1">
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="10543833" y="6775060"/>
+          <a:ext cx="3981792" cy="1845065"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:miter lim="800000"/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" wrap="square" lIns="18288" tIns="18288" rIns="0" bIns="0" anchor="t" upright="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l" rtl="0">
+            <a:defRPr sz="1000"/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Calibri"/>
+              <a:ea typeface="Calibri"/>
+              <a:cs typeface="Calibri"/>
+            </a:rPr>
+            <a:t>package dao</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l" rtl="0">
+            <a:defRPr sz="1000"/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Calibri"/>
+              <a:ea typeface="Calibri"/>
+              <a:cs typeface="Calibri"/>
+            </a:rPr>
+            <a:t>class UserDAO</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l" rtl="0">
+            <a:defRPr sz="1000"/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="Calibri"/>
+              <a:cs typeface="Calibri"/>
+            </a:rPr>
+            <a:t>- mapper : ObjectMapper</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l" rtl="0">
+            <a:defRPr sz="1000"/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Calibri"/>
+              <a:ea typeface="Calibri"/>
+              <a:cs typeface="Calibri"/>
+            </a:rPr>
+            <a:t>+ void addUser(User user)</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l" rtl="0">
+            <a:defRPr sz="1000"/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Calibri"/>
+              <a:ea typeface="Calibri"/>
+              <a:cs typeface="Calibri"/>
+            </a:rPr>
+            <a:t>+ List&lt;User&gt; getAllUsers()</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l" rtl="0">
+            <a:defRPr sz="1000"/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Calibri"/>
+              <a:ea typeface="Calibri"/>
+              <a:cs typeface="Calibri"/>
+            </a:rPr>
+            <a:t>+ User getUserById(String userId)</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l" rtl="0">
+            <a:defRPr sz="1000"/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Calibri"/>
+              <a:ea typeface="Calibri"/>
+              <a:cs typeface="Calibri"/>
+            </a:rPr>
+            <a:t>+ void printBorrowedBooks(User user)</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l" rtl="0">
+            <a:defRPr sz="1000"/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Calibri"/>
+              <a:ea typeface="Calibri"/>
+              <a:cs typeface="Calibri"/>
+            </a:rPr>
+            <a:t>+ void updateUser(User user)</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l" rtl="0">
+            <a:defRPr sz="1000"/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="Calibri"/>
+              <a:cs typeface="Calibri"/>
+            </a:rPr>
+            <a:t>- serializeBorrowedBooks(borrowedBookIds: List&lt;String&gt;) : String</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l" rtl="0">
+            <a:defRPr sz="1000"/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="Calibri"/>
+              <a:cs typeface="Calibri"/>
+            </a:rPr>
+            <a:t>- deserializeBorrowedBooks(json: String) : List&lt;String&gt;</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>282383</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>166688</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>28</xdr:col>
+      <xdr:colOff>358583</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>14288</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="3079" name="Text Box 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{34A9CCD5-A592-F6B2-A36D-A8E55086E3AF}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1">
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="15462852" y="5881688"/>
+          <a:ext cx="1897856" cy="800100"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:miter lim="800000"/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" wrap="square" lIns="18288" tIns="18288" rIns="0" bIns="0" anchor="t" upright="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l" rtl="0">
+            <a:defRPr sz="1000"/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Calibri"/>
+              <a:ea typeface="Calibri"/>
+              <a:cs typeface="Calibri"/>
+            </a:rPr>
+            <a:t>package service</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l" rtl="0">
+            <a:defRPr sz="1000"/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Calibri"/>
+              <a:ea typeface="Calibri"/>
+              <a:cs typeface="Calibri"/>
+            </a:rPr>
+            <a:t>class DBHelper</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l" rtl="0">
+            <a:defRPr sz="1000"/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Calibri"/>
+              <a:ea typeface="Calibri"/>
+              <a:cs typeface="Calibri"/>
+            </a:rPr>
+            <a:t>+ static Connection connect()</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l" rtl="0">
+            <a:defRPr sz="1000"/>
+          </a:pPr>
+          <a:endParaRPr lang="en-GB" sz="1100" b="0" i="0" u="none" strike="noStrike" baseline="0">
+            <a:solidFill>
+              <a:srgbClr val="000000"/>
+            </a:solidFill>
+            <a:latin typeface="Calibri"/>
+            <a:ea typeface="Calibri"/>
+            <a:cs typeface="Calibri"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>452437</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>61585</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>31</xdr:col>
+      <xdr:colOff>567394</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>153550</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="3080" name="Text Box 8">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{65E94FC0-85CA-2E57-31E2-42CE0CC80F5A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1">
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="15025687" y="442585"/>
+          <a:ext cx="4365488" cy="2568465"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:miter lim="800000"/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="18288" rIns="0" bIns="0" anchor="t" upright="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l" rtl="0">
+            <a:defRPr sz="1000"/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Calibri"/>
+              <a:ea typeface="Calibri"/>
+              <a:cs typeface="Calibri"/>
+            </a:rPr>
+            <a:t>package service</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l" rtl="0">
+            <a:defRPr sz="1000"/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Calibri"/>
+              <a:ea typeface="Calibri"/>
+              <a:cs typeface="Calibri"/>
+            </a:rPr>
+            <a:t>class LibraryManager</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l" rtl="0">
+            <a:defRPr sz="1000"/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Calibri"/>
+              <a:ea typeface="Calibri"/>
+              <a:cs typeface="Calibri"/>
+            </a:rPr>
+            <a:t>- UserDAO userDAO</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l" rtl="0">
+            <a:defRPr sz="1000"/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Calibri"/>
+              <a:ea typeface="Calibri"/>
+              <a:cs typeface="Calibri"/>
+            </a:rPr>
+            <a:t>- BookDAO bookDAO</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l" rtl="0">
+            <a:defRPr sz="1000"/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Calibri"/>
+              <a:ea typeface="Calibri"/>
+              <a:cs typeface="Calibri"/>
+            </a:rPr>
+            <a:t>- RecordDAO recordDAO</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l" rtl="0">
+            <a:defRPr sz="1000"/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Calibri"/>
+              <a:ea typeface="Calibri"/>
+              <a:cs typeface="Calibri"/>
+            </a:rPr>
+            <a:t>+ LibraryManager(UserDAO userDAO, BookDAO bookDAO, RecordDAO recordDAO)</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l" rtl="0">
+            <a:defRPr sz="1000"/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Calibri"/>
+              <a:ea typeface="Calibri"/>
+              <a:cs typeface="Calibri"/>
+            </a:rPr>
+            <a:t>+ void registerUser(User user)</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l" rtl="0">
+            <a:defRPr sz="1000"/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Calibri"/>
+              <a:ea typeface="Calibri"/>
+              <a:cs typeface="Calibri"/>
+            </a:rPr>
+            <a:t>+ void removeBook(Book book)</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l" rtl="0">
+            <a:defRPr sz="1000"/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Calibri"/>
+              <a:ea typeface="Calibri"/>
+              <a:cs typeface="Calibri"/>
+            </a:rPr>
+            <a:t>+ void addBook(Book book)</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l" rtl="0">
+            <a:defRPr sz="1000"/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Calibri"/>
+              <a:ea typeface="Calibri"/>
+              <a:cs typeface="Calibri"/>
+            </a:rPr>
+            <a:t>+ void borrowBook(String userId, String bookId)</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l" rtl="0">
+            <a:defRPr sz="1000"/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Calibri"/>
+              <a:ea typeface="Calibri"/>
+              <a:cs typeface="Calibri"/>
+            </a:rPr>
+            <a:t>+ void returnBook(String userId, String bookId)</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l" rtl="0">
+            <a:defRPr sz="1000"/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Calibri"/>
+              <a:ea typeface="Calibri"/>
+              <a:cs typeface="Calibri"/>
+            </a:rPr>
+            <a:t>+ void printAllRecords()</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l" rtl="0">
+            <a:defRPr sz="1000"/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Calibri"/>
+              <a:ea typeface="Calibri"/>
+              <a:cs typeface="Calibri"/>
+            </a:rPr>
+            <a:t>- String generateRecordId()</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l" rtl="0">
+            <a:defRPr sz="1000"/>
+          </a:pPr>
+          <a:endParaRPr lang="en-GB" sz="1100" b="0" i="0" u="none" strike="noStrike" baseline="0">
+            <a:solidFill>
+              <a:srgbClr val="000000"/>
+            </a:solidFill>
+            <a:latin typeface="Calibri"/>
+            <a:ea typeface="Calibri"/>
+            <a:cs typeface="Calibri"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>29</xdr:col>
+      <xdr:colOff>565753</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>80963</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>31</xdr:col>
+      <xdr:colOff>95250</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>11906</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="15" name="Text Box 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{618AB131-6CD3-4A78-B559-B5B3AF3389A0}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1">
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="18175097" y="6176963"/>
+          <a:ext cx="743934" cy="311943"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:miter lim="800000"/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" wrap="square" lIns="18288" tIns="18288" rIns="0" bIns="0" anchor="t" upright="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l" rtl="0">
+            <a:defRPr sz="1000"/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Calibri"/>
+              <a:ea typeface="Calibri"/>
+              <a:cs typeface="Calibri"/>
+            </a:rPr>
+            <a:t>SQLiteDB</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>557675</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>189507</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>282383</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>185738</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="17" name="Connector: Elbow 16">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1E1DDFAB-0564-4B25-7737-B02675AD1DF5}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="3076" idx="3"/>
+          <a:endCxn id="3079" idx="1"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="14523706" y="4761507"/>
+          <a:ext cx="939146" cy="1520231"/>
+        </a:xfrm>
+        <a:prstGeom prst="bentConnector3">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="dk1"/>
+          </a:solidFill>
+          <a:prstDash val="dash"/>
+          <a:round/>
+          <a:headEnd type="none" w="med" len="med"/>
+          <a:tailEnd type="none" w="med" len="med"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>94840</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>66430</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>282383</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>185738</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="19" name="Connector: Elbow 18">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9988D135-46CA-4A58-879C-03DB55F74964}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="3077" idx="3"/>
+          <a:endCxn id="3079" idx="1"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="12846434" y="6162430"/>
+          <a:ext cx="2616418" cy="119308"/>
+        </a:xfrm>
+        <a:prstGeom prst="bentConnector3">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 50000"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="dk1"/>
+          </a:solidFill>
+          <a:prstDash val="dash"/>
+          <a:round/>
+          <a:headEnd type="none" w="med" len="med"/>
+          <a:tailEnd type="none" w="med" len="med"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>559594</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>185738</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>282383</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>77593</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="22" name="Connector: Elbow 21">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EFDE6EE4-8FDD-4FF8-BAFA-5B1C8C3354E4}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="3078" idx="3"/>
+          <a:endCxn id="3079" idx="1"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="14525625" y="6281738"/>
+          <a:ext cx="937227" cy="1415855"/>
+        </a:xfrm>
+        <a:prstGeom prst="bentConnector3">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 50000"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="dk1"/>
+          </a:solidFill>
+          <a:prstDash val="dash"/>
+          <a:round/>
+          <a:headEnd type="none" w="med" len="med"/>
+          <a:tailEnd type="none" w="med" len="med"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>28</xdr:col>
+      <xdr:colOff>358583</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>185738</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>29</xdr:col>
+      <xdr:colOff>565753</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>46435</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="25" name="Connector: Elbow 24">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{529CA5EB-2274-40E6-8BCE-C244A0972EC2}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="3079" idx="3"/>
+          <a:endCxn id="15" idx="1"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="17360708" y="6281738"/>
+          <a:ext cx="814389" cy="51197"/>
+        </a:xfrm>
+        <a:prstGeom prst="bentConnector3">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="dk1"/>
+          </a:solidFill>
+          <a:prstDash val="dash"/>
+          <a:round/>
+          <a:headEnd type="none" w="med" len="med"/>
+          <a:tailEnd type="none" w="med" len="med"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
         </a:effectRef>
         <a:fontRef idx="minor">
           <a:schemeClr val="tx1"/>
@@ -1649,7 +4330,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="K10:T29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="W10" sqref="W10"/>
     </sheetView>
   </sheetViews>
@@ -1662,22 +4343,22 @@
     </row>
     <row r="26" spans="20:20" x14ac:dyDescent="0.25">
       <c r="T26" t="s">
-        <v>64</v>
+        <v>2</v>
       </c>
     </row>
     <row r="27" spans="20:20" x14ac:dyDescent="0.25">
       <c r="T27" t="s">
-        <v>65</v>
+        <v>3</v>
       </c>
     </row>
     <row r="28" spans="20:20" x14ac:dyDescent="0.25">
       <c r="T28" t="s">
-        <v>66</v>
+        <v>4</v>
       </c>
     </row>
     <row r="29" spans="20:20" x14ac:dyDescent="0.25">
       <c r="T29" t="s">
-        <v>15</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -1687,363 +4368,16 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3CD445AF-E16B-4187-BB5C-6DFAB2F0D563}">
-  <dimension ref="B2:O84"/>
-  <sheetViews>
-    <sheetView topLeftCell="A55" workbookViewId="0">
-      <selection activeCell="J21" sqref="J21"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="2" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B2" t="s">
-        <v>1</v>
-      </c>
-      <c r="O2" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="3" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B3" t="s">
-        <v>2</v>
-      </c>
-      <c r="O3" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="4" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B4" t="s">
-        <v>7</v>
-      </c>
-      <c r="O4" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="5" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B5" t="s">
-        <v>3</v>
-      </c>
-      <c r="O5" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="6" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B6" t="s">
-        <v>4</v>
-      </c>
-      <c r="O6" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="7" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B7" t="s">
-        <v>5</v>
-      </c>
-      <c r="O7" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="8" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B8" t="s">
-        <v>6</v>
-      </c>
-      <c r="O8" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="9" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="O9" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="10" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="O10" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="11" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="O11" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="12" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="D12" t="s">
-        <v>8</v>
-      </c>
-      <c r="O12" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="13" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="D13" t="s">
-        <v>9</v>
-      </c>
-      <c r="O13" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="14" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="D14" t="s">
-        <v>10</v>
-      </c>
-      <c r="O14" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="15" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="D15" t="s">
-        <v>11</v>
-      </c>
-      <c r="O15" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="16" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="D16" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="17" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D17" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="18" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D18" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="19" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D19" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="22" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D22" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="23" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D23" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="24" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D24" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="26" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D26" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="28" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D28" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="30" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D30" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="32" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D32" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="33" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D33" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="36" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D36" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="37" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D37" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="38" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D38" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="40" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D40" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="42" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D42" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="43" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D43" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="44" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D44" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="45" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D45" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="46" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D46" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="47" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D47" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="48" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D48" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="52" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D52" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="53" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D53" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="54" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D54" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="55" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D55" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="57" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D57" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="59" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D59" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="60" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D60" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="61" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D61" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="62" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D62" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="63" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D63" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="68" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D68" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="69" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D69" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="70" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D70" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="71" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D71" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="72" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D72" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="73" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D73" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="74" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D74" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="79" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D79" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="80" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D80" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="81" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D81" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="82" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D82" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="83" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D83" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="84" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D84" t="s">
-        <v>15</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C417AED-45C6-429C-BACE-0B63FAB20646}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{62CCAF17-2D6B-4E05-8263-F4BE9CCFCD56}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="AA27" sqref="AA27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>